<commit_message>
Move sensitivities to targets
</commit_message>
<xml_diff>
--- a/data/atlantic_salmon/params/Population.xlsx
+++ b/data/atlantic_salmon/params/Population.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\treimer\Documents\R-temp-files\local_to_global_mariculture_modelling\data\atlantic_salmon\params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F11DC35-8A12-4FDD-9A37-B0E6F6C55439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413158B3-1040-4217-810D-EE5AAF1FC29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7596" yWindow="1464" windowWidth="28236" windowHeight="14844" xr2:uid="{480EBA47-7647-41F2-86F2-E9AC7A875918}"/>
+    <workbookView xWindow="11712" yWindow="1176" windowWidth="24396" windowHeight="14844" xr2:uid="{480EBA47-7647-41F2-86F2-E9AC7A875918}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -119,7 +132,7 @@
     <t>SD overprovision of food</t>
   </si>
   <si>
-    <t>%</t>
+    <t>d-1</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1008,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>